<commit_message>
Converted function to class, fixed error with sheet indexes and updated code and readme.md
</commit_message>
<xml_diff>
--- a/example/output.xlsx
+++ b/example/output.xlsx
@@ -14,43 +14,49 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>Juanito Peréz</t>
-  </si>
-  <si>
-    <t>Edad</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Karl</t>
+  </si>
+  <si>
+    <t>Age</t>
   </si>
   <si>
     <t>24</t>
   </si>
   <si>
-    <t>Sexo</t>
-  </si>
-  <si>
-    <t>Hombre</t>
-  </si>
-  <si>
-    <t>Altura</t>
-  </si>
-  <si>
-    <t>1.74 metros</t>
-  </si>
-  <si>
-    <t>Peso</t>
-  </si>
-  <si>
-    <t>81 kg</t>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Man</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>1.78 m</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>72 kg</t>
+  </si>
+  <si>
+    <t>Uppercase name</t>
+  </si>
+  <si>
+    <t>KARL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -60,6 +66,13 @@
     </font>
     <font>
       <color rgb="FFFF0000"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <color rgb="FF0070C0"/>
       <family val="2"/>
       <scheme val="minor"/>
       <sz val="11"/>
@@ -101,9 +114,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" defaultColWidth="9.140625"/>
@@ -460,6 +474,14 @@
         <v>9</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>